<commit_message>
extracted market sentiments for 2010 - 2014
</commit_message>
<xml_diff>
--- a/sentiments.xlsx
+++ b/sentiments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D79"/>
+  <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,6 +451,16 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>message_content_z</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>message_content_a</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>message_content</t>
         </is>
       </c>
@@ -469,9 +479,15 @@
       <c r="C2" t="n">
         <v>0.8</v>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>0.8</t>
+      <c r="D2" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Positive</t>
         </is>
       </c>
     </row>
@@ -489,9 +505,15 @@
       <c r="C3" t="n">
         <v>0.1</v>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>0.2</t>
+      <c r="D3" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -509,9 +531,15 @@
       <c r="C4" t="n">
         <v>0.2</v>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>0.2</t>
+      <c r="D4" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -529,9 +557,15 @@
       <c r="C5" t="n">
         <v>0.2</v>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>0.1</t>
+      <c r="D5" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -549,9 +583,15 @@
       <c r="C6" t="n">
         <v>-0.6</v>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>-0.8</t>
+      <c r="D6" t="n">
+        <v>-0.8</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Negative</t>
         </is>
       </c>
     </row>
@@ -569,9 +609,15 @@
       <c r="C7" t="n">
         <v>0.2</v>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>-0.5</t>
+      <c r="D7" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -589,9 +635,15 @@
       <c r="C8" t="n">
         <v>0.3</v>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>0.3</t>
+      <c r="D8" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -609,9 +661,15 @@
       <c r="C9" t="n">
         <v>0.2</v>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -629,9 +687,15 @@
       <c r="C10" t="n">
         <v>0.8</v>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>0.8</t>
+      <c r="D10" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Positive</t>
         </is>
       </c>
     </row>
@@ -649,9 +713,15 @@
       <c r="C11" t="n">
         <v>0.5</v>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>0.2</t>
+      <c r="D11" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -669,9 +739,15 @@
       <c r="C12" t="n">
         <v>0.8</v>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>0.8</t>
+      <c r="D12" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Positive</t>
         </is>
       </c>
     </row>
@@ -689,9 +765,15 @@
       <c r="C13" t="n">
         <v>0.5</v>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>0.5</t>
+      <c r="D13" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Positive</t>
         </is>
       </c>
     </row>
@@ -709,9 +791,15 @@
       <c r="C14" t="n">
         <v>0.5</v>
       </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>0.5</t>
+      <c r="D14" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Positive</t>
         </is>
       </c>
     </row>
@@ -729,9 +817,15 @@
       <c r="C15" t="n">
         <v>0.2</v>
       </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>0.1</t>
+      <c r="D15" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -749,9 +843,15 @@
       <c r="C16" t="n">
         <v>0.1</v>
       </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>-0.3</t>
+      <c r="D16" t="n">
+        <v>-0.3</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -769,9 +869,15 @@
       <c r="C17" t="n">
         <v>0.6</v>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>0.5</t>
+      <c r="D17" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Positive</t>
         </is>
       </c>
     </row>
@@ -789,9 +895,15 @@
       <c r="C18" t="n">
         <v>0.6</v>
       </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>0.7</t>
+      <c r="D18" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Positive</t>
         </is>
       </c>
     </row>
@@ -809,9 +921,15 @@
       <c r="C19" t="n">
         <v>0.2</v>
       </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>0.1</t>
+      <c r="D19" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -829,9 +947,15 @@
       <c r="C20" t="n">
         <v>0.7</v>
       </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>0.6</t>
+      <c r="D20" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Positive</t>
         </is>
       </c>
     </row>
@@ -849,9 +973,15 @@
       <c r="C21" t="n">
         <v>0.2</v>
       </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -869,9 +999,15 @@
       <c r="C22" t="n">
         <v>0.3</v>
       </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -889,9 +1025,15 @@
       <c r="C23" t="n">
         <v>0.5</v>
       </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>0.1</t>
+      <c r="D23" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -909,9 +1051,15 @@
       <c r="C24" t="n">
         <v>0.7</v>
       </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>0.5</t>
+      <c r="D24" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -929,9 +1077,15 @@
       <c r="C25" t="n">
         <v>0.2</v>
       </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>-1</t>
+      <c r="D25" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E25" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Negative</t>
         </is>
       </c>
     </row>
@@ -949,9 +1103,15 @@
       <c r="C26" t="n">
         <v>0.2</v>
       </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D26" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -969,9 +1129,15 @@
       <c r="C27" t="n">
         <v>0.2</v>
       </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>-1</t>
+      <c r="D27" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -989,9 +1155,15 @@
       <c r="C28" t="n">
         <v>0.6</v>
       </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>0.7</t>
+      <c r="D28" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Positive</t>
         </is>
       </c>
     </row>
@@ -1009,9 +1181,15 @@
       <c r="C29" t="n">
         <v>0.5</v>
       </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>0.5</t>
+      <c r="D29" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Positive</t>
         </is>
       </c>
     </row>
@@ -1029,9 +1207,15 @@
       <c r="C30" t="n">
         <v>0.5</v>
       </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>0.7</t>
+      <c r="D30" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Positive</t>
         </is>
       </c>
     </row>
@@ -1049,9 +1233,15 @@
       <c r="C31" t="n">
         <v>0.6</v>
       </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>0.5</t>
+      <c r="D31" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Positive</t>
         </is>
       </c>
     </row>
@@ -1069,9 +1259,15 @@
       <c r="C32" t="n">
         <v>0.5</v>
       </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>0.3</t>
+      <c r="D32" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -1089,9 +1285,15 @@
       <c r="C33" t="n">
         <v>0.3</v>
       </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>0.1</t>
+      <c r="D33" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -1109,9 +1311,15 @@
       <c r="C34" t="n">
         <v>0.5</v>
       </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>0.2</t>
+      <c r="D34" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -1129,9 +1337,15 @@
       <c r="C35" t="n">
         <v>0.6</v>
       </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>0.6</t>
+      <c r="D35" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Positive</t>
         </is>
       </c>
     </row>
@@ -1149,9 +1363,15 @@
       <c r="C36" t="n">
         <v>-1</v>
       </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>-0.5</t>
+      <c r="D36" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="E36" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -1169,9 +1389,15 @@
       <c r="C37" t="n">
         <v>0.2</v>
       </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>0.2</t>
+      <c r="D37" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -1189,9 +1415,15 @@
       <c r="C38" t="n">
         <v>0.2</v>
       </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>0.2</t>
+      <c r="D38" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -1209,9 +1441,15 @@
       <c r="C39" t="n">
         <v>0.2</v>
       </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>0.3</t>
+      <c r="D39" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -1229,9 +1467,15 @@
       <c r="C40" t="n">
         <v>0</v>
       </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>-1</t>
+      <c r="D40" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -1249,9 +1493,15 @@
       <c r="C41" t="n">
         <v>-1</v>
       </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>-1</t>
+      <c r="D41" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E41" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Negative</t>
         </is>
       </c>
     </row>
@@ -1269,9 +1519,15 @@
       <c r="C42" t="n">
         <v>0.5</v>
       </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>0.5</t>
+      <c r="D42" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Positive</t>
         </is>
       </c>
     </row>
@@ -1289,9 +1545,15 @@
       <c r="C43" t="n">
         <v>0</v>
       </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>0.0</t>
+      <c r="D43" t="n">
+        <v>0</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0</v>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -1309,9 +1571,15 @@
       <c r="C44" t="n">
         <v>0.5</v>
       </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>-1</t>
+      <c r="D44" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0</v>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -1329,9 +1597,15 @@
       <c r="C45" t="n">
         <v>0.2</v>
       </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D45" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -1349,9 +1623,15 @@
       <c r="C46" t="n">
         <v>0.5</v>
       </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>0.5</t>
+      <c r="D46" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Positive</t>
         </is>
       </c>
     </row>
@@ -1369,9 +1649,15 @@
       <c r="C47" t="n">
         <v>0.2</v>
       </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>-0.5</t>
+      <c r="D47" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -1389,9 +1675,15 @@
       <c r="C48" t="n">
         <v>0.2</v>
       </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>0.5</t>
+      <c r="D48" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -1409,9 +1701,15 @@
       <c r="C49" t="n">
         <v>0.5</v>
       </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>0.5</t>
+      <c r="D49" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Positive</t>
         </is>
       </c>
     </row>
@@ -1429,9 +1727,15 @@
       <c r="C50" t="n">
         <v>0.6</v>
       </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>-1</t>
+      <c r="D50" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>neutral</t>
         </is>
       </c>
     </row>
@@ -1449,9 +1753,15 @@
       <c r="C51" t="n">
         <v>0.3</v>
       </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>0.2</t>
+      <c r="D51" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -1469,9 +1779,15 @@
       <c r="C52" t="n">
         <v>0.3</v>
       </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>0.2</t>
+      <c r="D52" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -1489,9 +1805,15 @@
       <c r="C53" t="n">
         <v>0.3</v>
       </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D53" t="n">
+        <v>0</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -1509,9 +1831,15 @@
       <c r="C54" t="n">
         <v>0.6</v>
       </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>0.6</t>
+      <c r="D54" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>Positive</t>
         </is>
       </c>
     </row>
@@ -1529,9 +1857,15 @@
       <c r="C55" t="n">
         <v>0.2</v>
       </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>0.2</t>
+      <c r="D55" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -1549,9 +1883,15 @@
       <c r="C56" t="n">
         <v>-0.3</v>
       </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>-0.5</t>
+      <c r="D56" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0</v>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Negative</t>
         </is>
       </c>
     </row>
@@ -1569,9 +1909,15 @@
       <c r="C57" t="n">
         <v>0.2</v>
       </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>0.5</t>
+      <c r="D57" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>Positive</t>
         </is>
       </c>
     </row>
@@ -1589,9 +1935,15 @@
       <c r="C58" t="n">
         <v>0</v>
       </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>-1</t>
+      <c r="D58" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E58" t="n">
+        <v>0</v>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -1609,9 +1961,15 @@
       <c r="C59" t="n">
         <v>0.6</v>
       </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>0.7</t>
+      <c r="D59" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="E59" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>Positive</t>
         </is>
       </c>
     </row>
@@ -1629,9 +1987,15 @@
       <c r="C60" t="n">
         <v>0.4</v>
       </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>0.5</t>
+      <c r="D60" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E60" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>Positive</t>
         </is>
       </c>
     </row>
@@ -1649,9 +2013,15 @@
       <c r="C61" t="n">
         <v>0.5</v>
       </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>0.2</t>
+      <c r="D61" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -1669,9 +2039,15 @@
       <c r="C62" t="n">
         <v>0.2</v>
       </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>-1</t>
+      <c r="D62" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E62" t="n">
+        <v>0</v>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -1689,9 +2065,15 @@
       <c r="C63" t="n">
         <v>0.2</v>
       </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>0.5</t>
+      <c r="D63" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E63" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -1709,9 +2091,15 @@
       <c r="C64" t="n">
         <v>0.8</v>
       </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>0.8</t>
+      <c r="D64" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="E64" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>Positive</t>
         </is>
       </c>
     </row>
@@ -1729,9 +2117,15 @@
       <c r="C65" t="n">
         <v>0.1</v>
       </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>0.2</t>
+      <c r="D65" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E65" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -1749,9 +2143,15 @@
       <c r="C66" t="n">
         <v>0.3</v>
       </c>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>0.2</t>
+      <c r="D66" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E66" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>Positive</t>
         </is>
       </c>
     </row>
@@ -1769,9 +2169,15 @@
       <c r="C67" t="n">
         <v>0.8</v>
       </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>0.8</t>
+      <c r="D67" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="E67" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>Positive</t>
         </is>
       </c>
     </row>
@@ -1789,9 +2195,15 @@
       <c r="C68" t="n">
         <v>0.7</v>
       </c>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>0.8</t>
+      <c r="D68" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="E68" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>Positive</t>
         </is>
       </c>
     </row>
@@ -1809,9 +2221,15 @@
       <c r="C69" t="n">
         <v>0.7</v>
       </c>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>0.6</t>
+      <c r="D69" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="E69" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -1829,9 +2247,15 @@
       <c r="C70" t="n">
         <v>-0.5</v>
       </c>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t>-0.5</t>
+      <c r="D70" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="E70" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>Negative</t>
         </is>
       </c>
     </row>
@@ -1849,9 +2273,15 @@
       <c r="C71" t="n">
         <v>0.1</v>
       </c>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>-0.2</t>
+      <c r="D71" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="E71" t="n">
+        <v>0</v>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -1869,9 +2299,15 @@
       <c r="C72" t="n">
         <v>0.5</v>
       </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>0.2</t>
+      <c r="D72" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E72" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>Positive</t>
         </is>
       </c>
     </row>
@@ -1889,9 +2325,15 @@
       <c r="C73" t="n">
         <v>0.8</v>
       </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>0.7</t>
+      <c r="D73" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="E73" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>Positive</t>
         </is>
       </c>
     </row>
@@ -1909,9 +2351,15 @@
       <c r="C74" t="n">
         <v>0.5</v>
       </c>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t>0.5</t>
+      <c r="D74" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E74" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>Positive</t>
         </is>
       </c>
     </row>
@@ -1929,9 +2377,15 @@
       <c r="C75" t="n">
         <v>0.3</v>
       </c>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>0.5</t>
+      <c r="D75" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E75" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -1949,9 +2403,15 @@
       <c r="C76" t="n">
         <v>0.6</v>
       </c>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t>0.8</t>
+      <c r="D76" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="E76" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>Positive</t>
         </is>
       </c>
     </row>
@@ -1969,9 +2429,15 @@
       <c r="C77" t="n">
         <v>0.5</v>
       </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>0.7</t>
+      <c r="D77" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="E77" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -1989,9 +2455,15 @@
       <c r="C78" t="n">
         <v>0.1</v>
       </c>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t>-0.5</t>
+      <c r="D78" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="E78" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -2009,9 +2481,15 @@
       <c r="C79" t="n">
         <v>0.2</v>
       </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>-0.5</t>
+      <c r="D79" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="E79" t="n">
+        <v>0</v>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>Neutral</t>
         </is>
       </c>
     </row>

</xml_diff>